<commit_message>
Fixed a couple pieces of info
</commit_message>
<xml_diff>
--- a/Papers/Chang 2006/Chang 2006.xlsx
+++ b/Papers/Chang 2006/Chang 2006.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="9860" yWindow="0" windowWidth="27300" windowHeight="15760"/>
+    <workbookView xWindow="560" yWindow="560" windowWidth="25040" windowHeight="15500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -567,7 +567,7 @@
   <dimension ref="A1:AW40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="E26" activeCellId="1" sqref="A39 E26"/>
+      <selection activeCell="AS21" sqref="AS21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2353,148 +2353,148 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="C15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="D15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="E15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="F15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="G15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="H15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="I15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="J15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="K15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="L15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="M15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="N15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="O15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="P15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="Q15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="R15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="S15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="T15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="U15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="V15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="W15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="X15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="Y15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="Z15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AA15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AB15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AC15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AD15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AE15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AF15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AG15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AH15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AI15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AJ15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AK15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AL15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AM15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AN15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AO15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AP15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AQ15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AR15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AS15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AT15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AU15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AV15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="AW15" s="2">
-        <v>30</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="16" spans="1:49">

</xml_diff>